<commit_message>
Adding emissions, adding storage start levels, a range of smaller improvements and fixes
</commit_message>
<xml_diff>
--- a/src_files/data_files/emissiondata_maf2020.xlsx
+++ b/src_files/data_files/emissiondata_maf2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BB\bb-master\north_european_model\src_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BB\bb-master\north_european_model\src_files\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462F92A6-C5B5-4F01-BE41-239D69C505B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FD63B2-ACC0-440B-8D22-7484019CD873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{3E3DEAD5-6055-4DB8-B424-EEC0B5E366CE}"/>
+    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="17520" xr2:uid="{3E3DEAD5-6055-4DB8-B424-EEC0B5E366CE}"/>
   </bookViews>
   <sheets>
     <sheet name="emissiondata" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <definedName name="Bottom">OFFSET(#REF!,1,0,COUNT(#REF!),1)</definedName>
     <definedName name="Labels">OFFSET(Bottom,0,-1)</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>CO2</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>Scenario</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>ETS_CO2</t>
   </si>
 </sst>
 </file>
@@ -454,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6EE8876-E835-4A4A-890C-1021AFC844BB}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -465,7 +471,7 @@
     <col min="1" max="1" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -476,10 +482,13 @@
         <v>5</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -489,11 +498,14 @@
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2">
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -503,11 +515,14 @@
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -517,11 +532,14 @@
       <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4">
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -531,7 +549,10 @@
       <c r="C5" t="s">
         <v>0</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5">
         <v>105</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New scenario "H2 balanced" that removes electricity shortages in "H2 heavy" scenario by restoring old thermal power plants (present in TYNDP 2020 NT 2025 scenario) while keeping everything else the same as in "H2 heavy".
</commit_message>
<xml_diff>
--- a/src_files/data_files/emissiondata_maf2020.xlsx
+++ b/src_files/data_files/emissiondata_maf2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BB\bb-master\north_european_model\src_files\data_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\backbone\north_european_model (2IMatch)\src_files\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FD63B2-ACC0-440B-8D22-7484019CD873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F179088E-D1A1-4C68-8628-5FD6521BD4DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="17520" xr2:uid="{3E3DEAD5-6055-4DB8-B424-EEC0B5E366CE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{3E3DEAD5-6055-4DB8-B424-EEC0B5E366CE}"/>
   </bookViews>
   <sheets>
     <sheet name="emissiondata" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>CO2</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>ETS_CO2</t>
+  </si>
+  <si>
+    <t>H2 balanced</t>
   </si>
 </sst>
 </file>
@@ -460,18 +463,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6EE8876-E835-4A4A-890C-1021AFC844BB}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" customWidth="1"/>
+    <col min="1" max="1" width="24.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -488,7 +491,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -505,7 +508,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -522,7 +525,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -539,7 +542,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -553,6 +556,23 @@
         <v>9</v>
       </c>
       <c r="E5">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>2035</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6">
         <v>105</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Banning underscore in user given names in e.g. units and groups, fixing a range of possible errors when merging data from multiple excels, introducing different merge methods: replace (default), add, multiply, and remove
</commit_message>
<xml_diff>
--- a/src_files/data_files/emissiondata_maf2020.xlsx
+++ b/src_files/data_files/emissiondata_maf2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BB\bb-master\north_european_model\src_files\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FD63B2-ACC0-440B-8D22-7484019CD873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD44A64B-3EFD-42AD-A02C-6548C167DF77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="17520" xr2:uid="{3E3DEAD5-6055-4DB8-B424-EEC0B5E366CE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{3E3DEAD5-6055-4DB8-B424-EEC0B5E366CE}"/>
   </bookViews>
   <sheets>
     <sheet name="emissiondata" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
     <t>group</t>
   </si>
   <si>
-    <t>ETS_CO2</t>
+    <t>ETS-CO2</t>
   </si>
 </sst>
 </file>

</xml_diff>